<commit_message>
add time cancel online booking setting
</commit_message>
<xml_diff>
--- a/src/models/data/global_setting.xlsx
+++ b/src/models/data/global_setting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE77091-E6D7-48D7-B3D8-CCA25D4DB582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E84934-0557-48CD-8088-9B0F5BEA79E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Số ngày cần phải tạo lịch biểu trước</t>
+  </si>
+  <si>
+    <t>771a7a56-6da0-4840-998a-f6e131310dda</t>
+  </si>
+  <si>
+    <t>cancelOnlineBookingAfterMinute</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Số phút hủy lịch đặt online</t>
   </si>
 </sst>
 </file>
@@ -403,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,6 +499,20 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>